<commit_message>
[IMP] Adjust SLA Procurement
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_sla_procurement.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_sla_procurement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SLA Procurement Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -1498,11 +1498,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="#,##0_);\(#,##0\)"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
+    <numFmt numFmtId="168" formatCode="#,##0"/>
+    <numFmt numFmtId="169" formatCode="#,##0_);\(#,##0\)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1602,7 +1604,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1619,16 +1621,24 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1647,7 +1657,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1671,6 +1681,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1679,11 +1693,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1792,66 +1806,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="20.6377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.6377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.0459183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="17.0459183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="16.9183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="20.4030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="15"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="3" width="18"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="4" width="18"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="15.234693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="6" width="13.4336734693878"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="20.0408163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="13.8061224489796"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="6" width="13.8061224489796"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="14.280612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="7" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="7" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="17.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="20.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="5" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="15.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="20.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="8" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="7" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="9" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="9" width="11.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="9" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8"/>
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10"/>
       <c r="D1" s="2"/>
       <c r="F1" s="1"/>
       <c r="K1" s="2"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="6"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="7"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
-      <c r="D2" s="9"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="0"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
-      <c r="K2" s="9"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="0"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="12"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="14"/>
       <c r="O2" s="0"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="12"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="14"/>
       <c r="R2" s="0"/>
       <c r="S2" s="0"/>
       <c r="T2" s="0"/>
@@ -2861,27 +2874,27 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
-      <c r="K3" s="9"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="0"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="12"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="14"/>
       <c r="O3" s="0"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="12"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="14"/>
       <c r="R3" s="0"/>
       <c r="S3" s="0"/>
       <c r="T3" s="0"/>
@@ -3891,25 +3904,25 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="0"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
-      <c r="K4" s="9"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="0"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14"/>
       <c r="O4" s="0"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="12"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14"/>
       <c r="R4" s="0"/>
       <c r="S4" s="0"/>
       <c r="T4" s="0"/>
@@ -4919,27 +4932,27 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="0"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="0"/>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
       <c r="J5" s="0"/>
-      <c r="K5" s="9"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="0"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="14"/>
       <c r="O5" s="0"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="12"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14"/>
       <c r="R5" s="0"/>
       <c r="S5" s="0"/>
       <c r="T5" s="0"/>
@@ -5949,27 +5962,27 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="0"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="0"/>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
       <c r="J6" s="0"/>
-      <c r="K6" s="9"/>
+      <c r="K6" s="11"/>
       <c r="L6" s="0"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14"/>
       <c r="O6" s="0"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
       <c r="R6" s="0"/>
       <c r="S6" s="0"/>
       <c r="T6" s="0"/>
@@ -6979,25 +6992,25 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="0"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
-      <c r="K7" s="9"/>
+      <c r="K7" s="11"/>
       <c r="L7" s="0"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="12"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="14"/>
       <c r="O7" s="0"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="12"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
       <c r="R7" s="0"/>
       <c r="S7" s="0"/>
       <c r="T7" s="0"/>
@@ -8007,25 +8020,25 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="0"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
-      <c r="K8" s="9"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="0"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="12"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="14"/>
       <c r="O8" s="0"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="12"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="14"/>
       <c r="R8" s="0"/>
       <c r="S8" s="0"/>
       <c r="T8" s="0"/>
@@ -9035,25 +9048,25 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="0"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
       <c r="J9" s="0"/>
-      <c r="K9" s="9"/>
+      <c r="K9" s="11"/>
       <c r="L9" s="0"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="14"/>
       <c r="O9" s="0"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="12"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="14"/>
       <c r="R9" s="0"/>
       <c r="S9" s="0"/>
       <c r="T9" s="0"/>
@@ -10063,23 +10076,23 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="0"/>
       <c r="C10" s="0"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
       <c r="J10" s="0"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="0"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14"/>
       <c r="O10" s="0"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="12"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
       <c r="R10" s="0"/>
       <c r="S10" s="0"/>
       <c r="T10" s="0"/>
@@ -11088,58 +11101,58 @@
       <c r="AMI10" s="0"/>
       <c r="AMJ10" s="0"/>
     </row>
-    <row r="11" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+    <row r="11" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="O11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="20"/>
+      <c r="P11" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -11154,3072 +11167,3072 @@
   </sheetPr>
   <dimension ref="A1:B459"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="24.9540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="22.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="24.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="22.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="29"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="29"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="29"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="29"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="26"/>
+      <c r="B24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="26"/>
+      <c r="B26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="29" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="26"/>
+      <c r="B31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="26"/>
+      <c r="B32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="26"/>
+      <c r="B33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="26"/>
+      <c r="B34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="27" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="27" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="26"/>
+      <c r="B38" s="29"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="26"/>
+      <c r="B39" s="29"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="26"/>
+      <c r="B40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="26"/>
+      <c r="B41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="26"/>
+      <c r="B42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="27" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="30" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="26"/>
+      <c r="B46" s="29"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="26"/>
+      <c r="B47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="26"/>
+      <c r="B48" s="29"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="26"/>
+      <c r="B49" s="29"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="26" t="s">
+      <c r="A50" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="29" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="29" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="26"/>
+      <c r="B52" s="29"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B53" s="26"/>
+      <c r="B53" s="29"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="26"/>
+      <c r="B54" s="29"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="26" t="s">
+      <c r="A55" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B55" s="26"/>
+      <c r="B55" s="29"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="30" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="29" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B58" s="26" t="s">
+      <c r="B58" s="29" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="26"/>
+      <c r="B59" s="29"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="26"/>
+      <c r="B60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="26"/>
+      <c r="B61" s="29"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="26"/>
+      <c r="B62" s="29"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B63" s="26"/>
+      <c r="B63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="24" t="s">
+      <c r="A65" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B66" s="26"/>
+      <c r="B66" s="29"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="24" t="s">
+      <c r="A67" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B67" s="26"/>
+      <c r="B67" s="29"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24" t="s">
+      <c r="A68" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B68" s="26"/>
+      <c r="B68" s="29"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="24" t="s">
+      <c r="A69" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B69" s="26"/>
+      <c r="B69" s="29"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="24" t="s">
+      <c r="A70" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B70" s="26"/>
+      <c r="B70" s="29"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="27" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="24" t="s">
+      <c r="A72" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B72" s="24" t="s">
+      <c r="B72" s="27" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="26" t="s">
+      <c r="A73" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B73" s="26"/>
+      <c r="B73" s="29"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="26" t="s">
+      <c r="A74" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B74" s="26"/>
+      <c r="B74" s="29"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="26" t="s">
+      <c r="A75" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B75" s="26"/>
+      <c r="B75" s="29"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="26" t="s">
+      <c r="A76" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B76" s="26"/>
+      <c r="B76" s="29"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="26" t="s">
+      <c r="A77" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B77" s="26"/>
+      <c r="B77" s="29"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="26" t="s">
+      <c r="A78" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B78" s="26" t="s">
+      <c r="B78" s="29" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="26" t="s">
+      <c r="A79" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="29" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="26" t="s">
+      <c r="A80" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="26"/>
+      <c r="B80" s="29"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="26"/>
+      <c r="B81" s="29"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="26" t="s">
+      <c r="A82" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B82" s="26"/>
+      <c r="B82" s="29"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="26" t="s">
+      <c r="A83" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B83" s="26"/>
+      <c r="B83" s="29"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="26" t="s">
+      <c r="A84" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B84" s="26"/>
+      <c r="B84" s="29"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="26" t="s">
+      <c r="A85" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B85" s="26" t="s">
+      <c r="B85" s="29" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="26" t="s">
+      <c r="A86" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B86" s="26" t="s">
+      <c r="B86" s="29" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="26" t="s">
+      <c r="A87" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B87" s="26"/>
+      <c r="B87" s="29"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B88" s="26"/>
+      <c r="B88" s="29"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="26" t="s">
+      <c r="A89" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B89" s="26"/>
+      <c r="B89" s="29"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="26" t="s">
+      <c r="A90" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B90" s="26"/>
+      <c r="B90" s="29"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="26" t="s">
+      <c r="A91" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B91" s="26"/>
+      <c r="B91" s="29"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="24" t="s">
+      <c r="A92" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="24" t="s">
+      <c r="B92" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="24" t="s">
+      <c r="A93" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" s="27" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="24" t="s">
+      <c r="A94" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="B94" s="26"/>
+      <c r="B94" s="29"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="24" t="s">
+      <c r="A95" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B95" s="26"/>
+      <c r="B95" s="29"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="24" t="s">
+      <c r="A96" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B96" s="26"/>
+      <c r="B96" s="29"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="24" t="s">
+      <c r="A97" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B97" s="25" t="s">
+      <c r="B97" s="28" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="24" t="s">
+      <c r="A98" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B98" s="26"/>
+      <c r="B98" s="29"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="24" t="s">
+      <c r="A99" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="24" t="s">
+      <c r="A100" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B100" s="24" t="s">
+      <c r="B100" s="27" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="24" t="s">
+      <c r="A101" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B101" s="26"/>
+      <c r="B101" s="29"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="24" t="s">
+      <c r="A102" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B102" s="26"/>
+      <c r="B102" s="29"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="24" t="s">
+      <c r="A103" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="B103" s="26"/>
+      <c r="B103" s="29"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="26" t="s">
+      <c r="A104" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B104" s="27" t="s">
+      <c r="B104" s="30" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="26" t="s">
+      <c r="A105" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="B105" s="27" t="s">
+      <c r="B105" s="30" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="26" t="s">
+      <c r="A106" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="B106" s="26" t="s">
+      <c r="B106" s="29" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="26" t="s">
+      <c r="A107" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="29" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="26" t="s">
+      <c r="A108" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B108" s="26" t="s">
+      <c r="B108" s="29" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="26" t="s">
+      <c r="A109" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="B109" s="26"/>
+      <c r="B109" s="29"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="26" t="s">
+      <c r="A110" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="B110" s="26"/>
+      <c r="B110" s="29"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="26" t="s">
+      <c r="A111" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B111" s="26"/>
+      <c r="B111" s="29"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="26" t="s">
+      <c r="A112" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="B112" s="26"/>
+      <c r="B112" s="29"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="26" t="s">
+      <c r="A113" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="B113" s="26" t="s">
+      <c r="B113" s="29" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="26" t="s">
+      <c r="A114" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B114" s="26" t="s">
+      <c r="B114" s="29" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="26" t="s">
+      <c r="A115" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B115" s="26"/>
+      <c r="B115" s="29"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="26" t="s">
+      <c r="A116" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B116" s="26"/>
+      <c r="B116" s="29"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="26" t="s">
+      <c r="A117" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="B117" s="26"/>
+      <c r="B117" s="29"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="26" t="s">
+      <c r="A118" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B118" s="26"/>
+      <c r="B118" s="29"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="26" t="s">
+      <c r="A119" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B119" s="26"/>
+      <c r="B119" s="29"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="26" t="s">
+      <c r="A120" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B120" s="26" t="s">
+      <c r="B120" s="29" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="26" t="s">
+      <c r="A121" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="B121" s="26" t="s">
+      <c r="B121" s="29" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="24" t="s">
+      <c r="A122" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="B122" s="26"/>
+      <c r="B122" s="29"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="24" t="s">
+      <c r="A123" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="B123" s="26"/>
+      <c r="B123" s="29"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="24" t="s">
+      <c r="A124" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="B124" s="26"/>
+      <c r="B124" s="29"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="24" t="s">
+      <c r="A125" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="B125" s="26"/>
+      <c r="B125" s="29"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="24" t="s">
+      <c r="A126" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="B126" s="26"/>
+      <c r="B126" s="29"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="24" t="s">
+      <c r="A127" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="B127" s="24" t="s">
+      <c r="B127" s="27" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="24" t="s">
+      <c r="A128" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="B128" s="24" t="s">
+      <c r="B128" s="27" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="24" t="s">
+      <c r="A129" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="B129" s="26"/>
+      <c r="B129" s="29"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="24" t="s">
+      <c r="A130" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="B130" s="26"/>
+      <c r="B130" s="29"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="24" t="s">
+      <c r="A131" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="B131" s="25" t="s">
+      <c r="B131" s="28" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="24" t="s">
+      <c r="A132" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="B132" s="26"/>
+      <c r="B132" s="29"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="24" t="s">
+      <c r="A133" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="B133" s="25" t="s">
+      <c r="B133" s="28" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="26" t="s">
+      <c r="A134" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B134" s="26" t="s">
+      <c r="B134" s="29" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="26" t="s">
+      <c r="A135" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B135" s="26" t="s">
+      <c r="B135" s="29" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="26" t="s">
+      <c r="A136" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="B136" s="26"/>
+      <c r="B136" s="29"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="26" t="s">
+      <c r="A137" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B137" s="26"/>
+      <c r="B137" s="29"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="26" t="s">
+      <c r="A138" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B138" s="26"/>
+      <c r="B138" s="29"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="26" t="s">
+      <c r="A139" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B139" s="26"/>
+      <c r="B139" s="29"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="26" t="s">
+      <c r="A140" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="B140" s="26"/>
+      <c r="B140" s="29"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="26" t="s">
+      <c r="A141" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="B141" s="26" t="s">
+      <c r="B141" s="29" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="26" t="s">
+      <c r="A142" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="B142" s="26" t="s">
+      <c r="B142" s="29" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="26" t="s">
+      <c r="A143" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B143" s="26"/>
+      <c r="B143" s="29"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="26" t="s">
+      <c r="A144" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B144" s="26"/>
+      <c r="B144" s="29"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="26" t="s">
+      <c r="A145" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B145" s="26"/>
+      <c r="B145" s="29"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="26" t="s">
+      <c r="A146" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="B146" s="26"/>
+      <c r="B146" s="29"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="26" t="s">
+      <c r="A147" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="B147" s="26"/>
+      <c r="B147" s="29"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="26" t="s">
+      <c r="A148" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="B148" s="26" t="s">
+      <c r="B148" s="29" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="26" t="s">
+      <c r="A149" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="B149" s="26" t="s">
+      <c r="B149" s="29" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="26" t="s">
+      <c r="A150" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="B150" s="26"/>
+      <c r="B150" s="29"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="26" t="s">
+      <c r="A151" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="B151" s="26"/>
+      <c r="B151" s="29"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="26" t="s">
+      <c r="A152" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="B152" s="26"/>
+      <c r="B152" s="29"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="24" t="s">
+      <c r="A153" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="B153" s="26"/>
+      <c r="B153" s="29"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="24" t="s">
+      <c r="A154" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="B154" s="26"/>
+      <c r="B154" s="29"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="24" t="s">
+      <c r="A155" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="B155" s="24" t="s">
+      <c r="B155" s="27" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="24" t="s">
+      <c r="A156" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="B156" s="24" t="s">
+      <c r="B156" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="24" t="s">
+      <c r="A157" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="B157" s="26"/>
+      <c r="B157" s="29"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="24" t="s">
+      <c r="A158" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="B158" s="26"/>
+      <c r="B158" s="29"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="24" t="s">
+      <c r="A159" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="B159" s="26"/>
+      <c r="B159" s="29"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="24" t="s">
+      <c r="A160" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="B160" s="26"/>
+      <c r="B160" s="29"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="24" t="s">
+      <c r="A161" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="B161" s="26"/>
+      <c r="B161" s="29"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="24" t="s">
+      <c r="A162" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="B162" s="24" t="s">
+      <c r="B162" s="27" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="24" t="s">
+      <c r="A163" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="B163" s="24" t="s">
+      <c r="B163" s="27" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="24" t="s">
+      <c r="A164" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="B164" s="26"/>
+      <c r="B164" s="29"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="26" t="s">
+      <c r="A165" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="B165" s="26"/>
+      <c r="B165" s="29"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="26" t="s">
+      <c r="A166" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="B166" s="26"/>
+      <c r="B166" s="29"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="26" t="s">
+      <c r="A167" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="B167" s="26"/>
+      <c r="B167" s="29"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="26" t="s">
+      <c r="A168" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="B168" s="26"/>
+      <c r="B168" s="29"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="26" t="s">
+      <c r="A169" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="B169" s="26" t="s">
+      <c r="B169" s="29" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="26" t="s">
+      <c r="A170" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="B170" s="26" t="s">
+      <c r="B170" s="29" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="26" t="s">
+      <c r="A171" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="B171" s="26"/>
+      <c r="B171" s="29"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="26" t="s">
+      <c r="A172" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="B172" s="26"/>
+      <c r="B172" s="29"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="26" t="s">
+      <c r="A173" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="B173" s="26"/>
+      <c r="B173" s="29"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="26" t="s">
+      <c r="A174" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="B174" s="26"/>
+      <c r="B174" s="29"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="26" t="s">
+      <c r="A175" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="B175" s="26"/>
+      <c r="B175" s="29"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="26" t="s">
+      <c r="A176" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="B176" s="26" t="s">
+      <c r="B176" s="29" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="26" t="s">
+      <c r="A177" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="B177" s="26" t="s">
+      <c r="B177" s="29" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="26" t="s">
+      <c r="A178" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="B178" s="26"/>
+      <c r="B178" s="29"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="26" t="s">
+      <c r="A179" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="B179" s="26"/>
+      <c r="B179" s="29"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="26" t="s">
+      <c r="A180" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="B180" s="26"/>
+      <c r="B180" s="29"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="26" t="s">
+      <c r="A181" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="B181" s="26"/>
+      <c r="B181" s="29"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="26" t="s">
+      <c r="A182" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="B182" s="26"/>
+      <c r="B182" s="29"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="24" t="s">
+      <c r="A183" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="B183" s="24" t="s">
+      <c r="B183" s="27" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="24" t="s">
+      <c r="A184" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="B184" s="24" t="s">
+      <c r="B184" s="27" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="24" t="s">
+      <c r="A185" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="B185" s="26"/>
+      <c r="B185" s="29"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="24" t="s">
+      <c r="A186" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="B186" s="26"/>
+      <c r="B186" s="29"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="24" t="s">
+      <c r="A187" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="B187" s="26"/>
+      <c r="B187" s="29"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="24" t="s">
+      <c r="A188" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="B188" s="26"/>
+      <c r="B188" s="29"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="24" t="s">
+      <c r="A189" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="B189" s="26"/>
+      <c r="B189" s="29"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="24" t="s">
+      <c r="A190" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="B190" s="24" t="s">
+      <c r="B190" s="27" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="24" t="s">
+      <c r="A191" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="B191" s="24" t="s">
+      <c r="B191" s="27" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="24" t="s">
+      <c r="A192" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="B192" s="25" t="s">
+      <c r="B192" s="28" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="24" t="s">
+      <c r="A193" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="B193" s="26"/>
+      <c r="B193" s="29"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="24" t="s">
+      <c r="A194" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="B194" s="26"/>
+      <c r="B194" s="29"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="26" t="s">
+      <c r="A195" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="B195" s="26"/>
+      <c r="B195" s="29"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="26" t="s">
+      <c r="A196" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="B196" s="26"/>
+      <c r="B196" s="29"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="26" t="s">
+      <c r="A197" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="B197" s="26" t="s">
+      <c r="B197" s="29" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="26" t="s">
+      <c r="A198" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="B198" s="26" t="s">
+      <c r="B198" s="29" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="26" t="s">
+      <c r="A199" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="B199" s="26"/>
+      <c r="B199" s="29"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="26" t="s">
+      <c r="A200" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="B200" s="26"/>
+      <c r="B200" s="29"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="26" t="s">
+      <c r="A201" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="B201" s="26"/>
+      <c r="B201" s="29"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="26" t="s">
+      <c r="A202" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="B202" s="26"/>
+      <c r="B202" s="29"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="26" t="s">
+      <c r="A203" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="B203" s="26"/>
+      <c r="B203" s="29"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="26" t="s">
+      <c r="A204" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="B204" s="26" t="s">
+      <c r="B204" s="29" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="26" t="s">
+      <c r="A205" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="B205" s="26" t="s">
+      <c r="B205" s="29" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="26" t="s">
+      <c r="A206" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="B206" s="26"/>
+      <c r="B206" s="29"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="26" t="s">
+      <c r="A207" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="B207" s="26"/>
+      <c r="B207" s="29"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="26" t="s">
+      <c r="A208" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="B208" s="26"/>
+      <c r="B208" s="29"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="26" t="s">
+      <c r="A209" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="B209" s="26"/>
+      <c r="B209" s="29"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="26" t="s">
+      <c r="A210" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="B210" s="26" t="s">
+      <c r="B210" s="29" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="26" t="s">
+      <c r="A211" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="B211" s="26" t="s">
+      <c r="B211" s="29" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="26" t="s">
+      <c r="A212" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="B212" s="26" t="s">
+      <c r="B212" s="29" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="26" t="s">
+      <c r="A213" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="B213" s="26"/>
+      <c r="B213" s="29"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="24" t="s">
+      <c r="A214" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="B214" s="26"/>
+      <c r="B214" s="29"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="24" t="s">
+      <c r="A215" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="B215" s="26"/>
+      <c r="B215" s="29"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="24" t="s">
+      <c r="A216" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="B216" s="26"/>
+      <c r="B216" s="29"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="24" t="s">
+      <c r="A217" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="B217" s="26"/>
+      <c r="B217" s="29"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="24" t="s">
+      <c r="A218" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="B218" s="24" t="s">
+      <c r="B218" s="27" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="24" t="s">
+      <c r="A219" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="B219" s="24" t="s">
+      <c r="B219" s="27" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="24" t="s">
+      <c r="A220" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B220" s="26"/>
+      <c r="B220" s="29"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="24" t="s">
+      <c r="A221" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="B221" s="26"/>
+      <c r="B221" s="29"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="24" t="s">
+      <c r="A222" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="B222" s="26"/>
+      <c r="B222" s="29"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="24" t="s">
+      <c r="A223" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="B223" s="26"/>
+      <c r="B223" s="29"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="24" t="s">
+      <c r="A224" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="B224" s="26"/>
+      <c r="B224" s="29"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="24" t="s">
+      <c r="A225" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="B225" s="24" t="s">
+      <c r="B225" s="27" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="26" t="s">
+      <c r="A226" s="29" t="s">
         <v>250</v>
       </c>
-      <c r="B226" s="26" t="s">
+      <c r="B226" s="29" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="27" t="s">
+      <c r="A227" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="B227" s="27" t="s">
+      <c r="B227" s="30" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="26" t="s">
+      <c r="A228" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="B228" s="26"/>
+      <c r="B228" s="29"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="26" t="s">
+      <c r="A229" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="B229" s="26"/>
+      <c r="B229" s="29"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="26" t="s">
+      <c r="A230" s="29" t="s">
         <v>254</v>
       </c>
-      <c r="B230" s="26"/>
+      <c r="B230" s="29"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="26" t="s">
+      <c r="A231" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="B231" s="26"/>
+      <c r="B231" s="29"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="26" t="s">
+      <c r="A232" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="B232" s="26" t="s">
+      <c r="B232" s="29" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="26" t="s">
+      <c r="A233" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="B233" s="26" t="s">
+      <c r="B233" s="29" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="26" t="s">
+      <c r="A234" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="B234" s="26"/>
+      <c r="B234" s="29"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="26" t="s">
+      <c r="A235" s="29" t="s">
         <v>259</v>
       </c>
-      <c r="B235" s="26"/>
+      <c r="B235" s="29"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="26" t="s">
+      <c r="A236" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="B236" s="26"/>
+      <c r="B236" s="29"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="26" t="s">
+      <c r="A237" s="29" t="s">
         <v>261</v>
       </c>
-      <c r="B237" s="26"/>
+      <c r="B237" s="29"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="26" t="s">
+      <c r="A238" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="B238" s="26"/>
+      <c r="B238" s="29"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="26" t="s">
+      <c r="A239" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="B239" s="26" t="s">
+      <c r="B239" s="29" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="26" t="s">
+      <c r="A240" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="B240" s="26" t="s">
+      <c r="B240" s="29" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="26" t="s">
+      <c r="A241" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="B241" s="26"/>
+      <c r="B241" s="29"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="26" t="s">
+      <c r="A242" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="B242" s="26"/>
+      <c r="B242" s="29"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="26" t="s">
+      <c r="A243" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="B243" s="26"/>
+      <c r="B243" s="29"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="26" t="s">
+      <c r="A244" s="29" t="s">
         <v>268</v>
       </c>
-      <c r="B244" s="26"/>
+      <c r="B244" s="29"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="24" t="s">
+      <c r="A245" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="B245" s="26"/>
+      <c r="B245" s="29"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="24" t="s">
+      <c r="A246" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="B246" s="24" t="s">
+      <c r="B246" s="27" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="24" t="s">
+      <c r="A247" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="B247" s="24" t="s">
+      <c r="B247" s="27" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="24" t="s">
+      <c r="A248" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="B248" s="26"/>
+      <c r="B248" s="29"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="24" t="s">
+      <c r="A249" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="B249" s="26"/>
+      <c r="B249" s="29"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="24" t="s">
+      <c r="A250" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="B250" s="26"/>
+      <c r="B250" s="29"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="24" t="s">
+      <c r="A251" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="B251" s="26"/>
+      <c r="B251" s="29"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="24" t="s">
+      <c r="A252" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="B252" s="26"/>
+      <c r="B252" s="29"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="24" t="s">
+      <c r="A253" s="27" t="s">
         <v>277</v>
       </c>
-      <c r="B253" s="24" t="s">
+      <c r="B253" s="27" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="24" t="s">
+      <c r="A254" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="B254" s="24" t="s">
+      <c r="B254" s="27" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="24" t="s">
+      <c r="A255" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="B255" s="26"/>
+      <c r="B255" s="29"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="24" t="s">
+      <c r="A256" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="B256" s="26"/>
+      <c r="B256" s="29"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="26" t="s">
+      <c r="A257" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="B257" s="26"/>
+      <c r="B257" s="29"/>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="26" t="s">
+      <c r="A258" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="B258" s="26"/>
+      <c r="B258" s="29"/>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="26" t="s">
+      <c r="A259" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="B259" s="26"/>
+      <c r="B259" s="29"/>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="26" t="s">
+      <c r="A260" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="B260" s="26" t="s">
+      <c r="B260" s="29" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="26" t="s">
+      <c r="A261" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="B261" s="26" t="s">
+      <c r="B261" s="29" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="26" t="s">
+      <c r="A262" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="B262" s="26"/>
+      <c r="B262" s="29"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="26" t="s">
+      <c r="A263" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="B263" s="26"/>
+      <c r="B263" s="29"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="26" t="s">
+      <c r="A264" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="B264" s="26"/>
+      <c r="B264" s="29"/>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="26" t="s">
+      <c r="A265" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="B265" s="26"/>
+      <c r="B265" s="29"/>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="26" t="s">
+      <c r="A266" s="29" t="s">
         <v>290</v>
       </c>
-      <c r="B266" s="26"/>
+      <c r="B266" s="29"/>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="26" t="s">
+      <c r="A267" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="B267" s="26" t="s">
+      <c r="B267" s="29" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="26" t="s">
+      <c r="A268" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="B268" s="26" t="s">
+      <c r="B268" s="29" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="26" t="s">
+      <c r="A269" s="29" t="s">
         <v>293</v>
       </c>
-      <c r="B269" s="26"/>
+      <c r="B269" s="29"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="26" t="s">
+      <c r="A270" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="B270" s="26"/>
+      <c r="B270" s="29"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="26" t="s">
+      <c r="A271" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="B271" s="26"/>
+      <c r="B271" s="29"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="26" t="s">
+      <c r="A272" s="29" t="s">
         <v>296</v>
       </c>
-      <c r="B272" s="26"/>
+      <c r="B272" s="29"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="26" t="s">
+      <c r="A273" s="29" t="s">
         <v>297</v>
       </c>
-      <c r="B273" s="26"/>
+      <c r="B273" s="29"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="26" t="s">
+      <c r="A274" s="29" t="s">
         <v>298</v>
       </c>
-      <c r="B274" s="26" t="s">
+      <c r="B274" s="29" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="24" t="s">
+      <c r="A275" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="B275" s="24" t="s">
+      <c r="B275" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="24" t="s">
+      <c r="A276" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="B276" s="26"/>
+      <c r="B276" s="29"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="24" t="s">
+      <c r="A277" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="B277" s="26"/>
+      <c r="B277" s="29"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="24" t="s">
+      <c r="A278" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="B278" s="26"/>
+      <c r="B278" s="29"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="24" t="s">
+      <c r="A279" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="B279" s="26"/>
+      <c r="B279" s="29"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="24" t="s">
+      <c r="A280" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="B280" s="26"/>
+      <c r="B280" s="29"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="24" t="s">
+      <c r="A281" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="B281" s="24" t="s">
+      <c r="B281" s="27" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="24" t="s">
+      <c r="A282" s="27" t="s">
         <v>306</v>
       </c>
-      <c r="B282" s="24" t="s">
+      <c r="B282" s="27" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="24" t="s">
+      <c r="A283" s="27" t="s">
         <v>307</v>
       </c>
-      <c r="B283" s="26"/>
+      <c r="B283" s="29"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="24" t="s">
+      <c r="A284" s="27" t="s">
         <v>308</v>
       </c>
-      <c r="B284" s="26"/>
+      <c r="B284" s="29"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="24" t="s">
+      <c r="A285" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="B285" s="26"/>
+      <c r="B285" s="29"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="24" t="s">
+      <c r="A286" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="B286" s="26"/>
+      <c r="B286" s="29"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="26" t="s">
+      <c r="A287" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="B287" s="27" t="s">
+      <c r="B287" s="30" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="26" t="s">
+      <c r="A288" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="B288" s="26" t="s">
+      <c r="B288" s="29" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="26" t="s">
+      <c r="A289" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="B289" s="26" t="s">
+      <c r="B289" s="29" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="26" t="s">
+      <c r="A290" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="B290" s="26"/>
+      <c r="B290" s="29"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="26" t="s">
+      <c r="A291" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="B291" s="26"/>
+      <c r="B291" s="29"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="26" t="s">
+      <c r="A292" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="B292" s="26"/>
+      <c r="B292" s="29"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="26" t="s">
+      <c r="A293" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="B293" s="26"/>
+      <c r="B293" s="29"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="26" t="s">
+      <c r="A294" s="29" t="s">
         <v>318</v>
       </c>
-      <c r="B294" s="26"/>
+      <c r="B294" s="29"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="26" t="s">
+      <c r="A295" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="B295" s="26" t="s">
+      <c r="B295" s="29" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="26" t="s">
+      <c r="A296" s="29" t="s">
         <v>320</v>
       </c>
-      <c r="B296" s="26" t="s">
+      <c r="B296" s="29" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="26" t="s">
+      <c r="A297" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="B297" s="27" t="s">
+      <c r="B297" s="30" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="26" t="s">
+      <c r="A298" s="29" t="s">
         <v>322</v>
       </c>
-      <c r="B298" s="26"/>
+      <c r="B298" s="29"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="26" t="s">
+      <c r="A299" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="B299" s="26"/>
+      <c r="B299" s="29"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="26" t="s">
+      <c r="A300" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="B300" s="27" t="s">
+      <c r="B300" s="30" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="26" t="s">
+      <c r="A301" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="B301" s="26"/>
+      <c r="B301" s="29"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="26" t="s">
+      <c r="A302" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="B302" s="26" t="s">
+      <c r="B302" s="29" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="26" t="s">
+      <c r="A303" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="B303" s="26" t="s">
+      <c r="B303" s="29" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="26" t="s">
+      <c r="A304" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="B304" s="26"/>
+      <c r="B304" s="29"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="26" t="s">
+      <c r="A305" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="B305" s="26"/>
+      <c r="B305" s="29"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="24" t="s">
+      <c r="A306" s="27" t="s">
         <v>330</v>
       </c>
-      <c r="B306" s="26"/>
+      <c r="B306" s="29"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="24" t="s">
+      <c r="A307" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="B307" s="26"/>
+      <c r="B307" s="29"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="24" t="s">
+      <c r="A308" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="B308" s="26"/>
+      <c r="B308" s="29"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="24" t="s">
+      <c r="A309" s="27" t="s">
         <v>333</v>
       </c>
-      <c r="B309" s="24" t="s">
+      <c r="B309" s="27" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="24" t="s">
+      <c r="A310" s="27" t="s">
         <v>334</v>
       </c>
-      <c r="B310" s="24" t="s">
+      <c r="B310" s="27" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="24" t="s">
+      <c r="A311" s="27" t="s">
         <v>335</v>
       </c>
-      <c r="B311" s="26"/>
+      <c r="B311" s="29"/>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="24" t="s">
+      <c r="A312" s="27" t="s">
         <v>336</v>
       </c>
-      <c r="B312" s="26"/>
+      <c r="B312" s="29"/>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="24" t="s">
+      <c r="A313" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="B313" s="26"/>
+      <c r="B313" s="29"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="24" t="s">
+      <c r="A314" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="B314" s="26"/>
+      <c r="B314" s="29"/>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="24" t="s">
+      <c r="A315" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="B315" s="26"/>
+      <c r="B315" s="29"/>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="24" t="s">
+      <c r="A316" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="B316" s="24" t="s">
+      <c r="B316" s="27" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="24" t="s">
+      <c r="A317" s="27" t="s">
         <v>341</v>
       </c>
-      <c r="B317" s="24" t="s">
+      <c r="B317" s="27" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="26" t="s">
+      <c r="A318" s="29" t="s">
         <v>342</v>
       </c>
-      <c r="B318" s="26"/>
+      <c r="B318" s="29"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="26" t="s">
+      <c r="A319" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="B319" s="26"/>
+      <c r="B319" s="29"/>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="26" t="s">
+      <c r="A320" s="29" t="s">
         <v>344</v>
       </c>
-      <c r="B320" s="26"/>
+      <c r="B320" s="29"/>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="26" t="s">
+      <c r="A321" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="B321" s="26"/>
+      <c r="B321" s="29"/>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="26" t="s">
+      <c r="A322" s="29" t="s">
         <v>346</v>
       </c>
-      <c r="B322" s="26"/>
+      <c r="B322" s="29"/>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="26" t="s">
+      <c r="A323" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="B323" s="26" t="s">
+      <c r="B323" s="29" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="26" t="s">
+      <c r="A324" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="B324" s="26" t="s">
+      <c r="B324" s="29" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="26" t="s">
+      <c r="A325" s="29" t="s">
         <v>349</v>
       </c>
-      <c r="B325" s="26"/>
+      <c r="B325" s="29"/>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="26" t="s">
+      <c r="A326" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="B326" s="26"/>
+      <c r="B326" s="29"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="26" t="s">
+      <c r="A327" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="B327" s="26"/>
+      <c r="B327" s="29"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="26" t="s">
+      <c r="A328" s="29" t="s">
         <v>352</v>
       </c>
-      <c r="B328" s="26"/>
+      <c r="B328" s="29"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="26" t="s">
+      <c r="A329" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="B329" s="26"/>
+      <c r="B329" s="29"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="26" t="s">
+      <c r="A330" s="29" t="s">
         <v>354</v>
       </c>
-      <c r="B330" s="26" t="s">
+      <c r="B330" s="29" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="26" t="s">
+      <c r="A331" s="29" t="s">
         <v>355</v>
       </c>
-      <c r="B331" s="26" t="s">
+      <c r="B331" s="29" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="26" t="s">
+      <c r="A332" s="29" t="s">
         <v>356</v>
       </c>
-      <c r="B332" s="26"/>
+      <c r="B332" s="29"/>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="26" t="s">
+      <c r="A333" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="B333" s="26"/>
+      <c r="B333" s="29"/>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="26" t="s">
+      <c r="A334" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="B334" s="26"/>
+      <c r="B334" s="29"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="26" t="s">
+      <c r="A335" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="B335" s="26"/>
+      <c r="B335" s="29"/>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="24" t="s">
+      <c r="A336" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="B336" s="26"/>
+      <c r="B336" s="29"/>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="24" t="s">
+      <c r="A337" s="27" t="s">
         <v>361</v>
       </c>
-      <c r="B337" s="24" t="s">
+      <c r="B337" s="27" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="24" t="s">
+      <c r="A338" s="27" t="s">
         <v>362</v>
       </c>
-      <c r="B338" s="24" t="s">
+      <c r="B338" s="27" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="24" t="s">
+      <c r="A339" s="27" t="s">
         <v>363</v>
       </c>
-      <c r="B339" s="26"/>
+      <c r="B339" s="29"/>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="24" t="s">
+      <c r="A340" s="27" t="s">
         <v>364</v>
       </c>
-      <c r="B340" s="25" t="s">
+      <c r="B340" s="28" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="24" t="s">
+      <c r="A341" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="B341" s="26"/>
+      <c r="B341" s="29"/>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="24" t="s">
+      <c r="A342" s="27" t="s">
         <v>366</v>
       </c>
-      <c r="B342" s="26"/>
+      <c r="B342" s="29"/>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="24" t="s">
+      <c r="A343" s="27" t="s">
         <v>367</v>
       </c>
-      <c r="B343" s="26"/>
+      <c r="B343" s="29"/>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="24" t="s">
+      <c r="A344" s="27" t="s">
         <v>368</v>
       </c>
-      <c r="B344" s="24" t="s">
+      <c r="B344" s="27" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="24" t="s">
+      <c r="A345" s="27" t="s">
         <v>369</v>
       </c>
-      <c r="B345" s="24" t="s">
+      <c r="B345" s="27" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="24" t="s">
+      <c r="A346" s="27" t="s">
         <v>370</v>
       </c>
-      <c r="B346" s="25" t="s">
+      <c r="B346" s="28" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="24" t="s">
+      <c r="A347" s="27" t="s">
         <v>371</v>
       </c>
-      <c r="B347" s="26"/>
+      <c r="B347" s="29"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="26" t="s">
+      <c r="A348" s="29" t="s">
         <v>372</v>
       </c>
-      <c r="B348" s="26"/>
+      <c r="B348" s="29"/>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="26" t="s">
+      <c r="A349" s="29" t="s">
         <v>373</v>
       </c>
-      <c r="B349" s="26"/>
+      <c r="B349" s="29"/>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="26" t="s">
+      <c r="A350" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="B350" s="26"/>
+      <c r="B350" s="29"/>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="26" t="s">
+      <c r="A351" s="29" t="s">
         <v>375</v>
       </c>
-      <c r="B351" s="26" t="s">
+      <c r="B351" s="29" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="26" t="s">
+      <c r="A352" s="29" t="s">
         <v>376</v>
       </c>
-      <c r="B352" s="26" t="s">
+      <c r="B352" s="29" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="26" t="s">
+      <c r="A353" s="29" t="s">
         <v>377</v>
       </c>
-      <c r="B353" s="26"/>
+      <c r="B353" s="29"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="26" t="s">
+      <c r="A354" s="29" t="s">
         <v>378</v>
       </c>
-      <c r="B354" s="26"/>
+      <c r="B354" s="29"/>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="26" t="s">
+      <c r="A355" s="29" t="s">
         <v>379</v>
       </c>
-      <c r="B355" s="26"/>
+      <c r="B355" s="29"/>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="26" t="s">
+      <c r="A356" s="29" t="s">
         <v>380</v>
       </c>
-      <c r="B356" s="26"/>
+      <c r="B356" s="29"/>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="26" t="s">
+      <c r="A357" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="B357" s="26"/>
+      <c r="B357" s="29"/>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="26" t="s">
+      <c r="A358" s="29" t="s">
         <v>382</v>
       </c>
-      <c r="B358" s="26" t="s">
+      <c r="B358" s="29" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="26" t="s">
+      <c r="A359" s="29" t="s">
         <v>383</v>
       </c>
-      <c r="B359" s="26" t="s">
+      <c r="B359" s="29" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="26" t="s">
+      <c r="A360" s="29" t="s">
         <v>384</v>
       </c>
-      <c r="B360" s="26"/>
+      <c r="B360" s="29"/>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="26" t="s">
+      <c r="A361" s="29" t="s">
         <v>385</v>
       </c>
-      <c r="B361" s="26"/>
+      <c r="B361" s="29"/>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="26" t="s">
+      <c r="A362" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="B362" s="26"/>
+      <c r="B362" s="29"/>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="26" t="s">
+      <c r="A363" s="29" t="s">
         <v>387</v>
       </c>
-      <c r="B363" s="26"/>
+      <c r="B363" s="29"/>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="26" t="s">
+      <c r="A364" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="B364" s="26"/>
+      <c r="B364" s="29"/>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="26" t="s">
+      <c r="A365" s="29" t="s">
         <v>389</v>
       </c>
-      <c r="B365" s="26" t="s">
+      <c r="B365" s="29" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="26" t="s">
+      <c r="A366" s="29" t="s">
         <v>390</v>
       </c>
-      <c r="B366" s="26" t="s">
+      <c r="B366" s="29" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="24" t="s">
+      <c r="A367" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="B367" s="24" t="s">
+      <c r="B367" s="27" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="24" t="s">
+      <c r="A368" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="B368" s="24" t="s">
+      <c r="B368" s="27" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="24" t="s">
+      <c r="A369" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="B369" s="26"/>
+      <c r="B369" s="29"/>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="24" t="s">
+      <c r="A370" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="B370" s="26"/>
+      <c r="B370" s="29"/>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="24" t="s">
+      <c r="A371" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="B371" s="26"/>
+      <c r="B371" s="29"/>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="24" t="s">
+      <c r="A372" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="B372" s="25" t="s">
+      <c r="B372" s="28" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="24" t="s">
+      <c r="A373" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="B373" s="25" t="s">
+      <c r="B373" s="28" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="24" t="s">
+      <c r="A374" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="B374" s="26"/>
+      <c r="B374" s="29"/>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="24" t="s">
+      <c r="A375" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="B375" s="26"/>
+      <c r="B375" s="29"/>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="24" t="s">
+      <c r="A376" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="B376" s="26"/>
+      <c r="B376" s="29"/>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="24" t="s">
+      <c r="A377" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="B377" s="26"/>
+      <c r="B377" s="29"/>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="24" t="s">
+      <c r="A378" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="B378" s="26"/>
+      <c r="B378" s="29"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="26" t="s">
+      <c r="A379" s="29" t="s">
         <v>403</v>
       </c>
-      <c r="B379" s="27" t="s">
+      <c r="B379" s="30" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="26" t="s">
+      <c r="A380" s="29" t="s">
         <v>404</v>
       </c>
-      <c r="B380" s="27" t="s">
+      <c r="B380" s="30" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="26" t="s">
+      <c r="A381" s="29" t="s">
         <v>405</v>
       </c>
-      <c r="B381" s="26"/>
+      <c r="B381" s="29"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="26" t="s">
+      <c r="A382" s="29" t="s">
         <v>406</v>
       </c>
-      <c r="B382" s="26"/>
+      <c r="B382" s="29"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="26" t="s">
+      <c r="A383" s="29" t="s">
         <v>407</v>
       </c>
-      <c r="B383" s="26"/>
+      <c r="B383" s="29"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="26" t="s">
+      <c r="A384" s="29" t="s">
         <v>408</v>
       </c>
-      <c r="B384" s="26"/>
+      <c r="B384" s="29"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="26" t="s">
+      <c r="A385" s="29" t="s">
         <v>409</v>
       </c>
-      <c r="B385" s="26"/>
+      <c r="B385" s="29"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="26" t="s">
+      <c r="A386" s="29" t="s">
         <v>410</v>
       </c>
-      <c r="B386" s="27" t="s">
+      <c r="B386" s="30" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="26" t="s">
+      <c r="A387" s="29" t="s">
         <v>411</v>
       </c>
-      <c r="B387" s="27" t="s">
+      <c r="B387" s="30" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="26" t="s">
+      <c r="A388" s="29" t="s">
         <v>412</v>
       </c>
-      <c r="B388" s="26"/>
+      <c r="B388" s="29"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="26" t="s">
+      <c r="A389" s="29" t="s">
         <v>413</v>
       </c>
-      <c r="B389" s="26"/>
+      <c r="B389" s="29"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="26" t="s">
+      <c r="A390" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="B390" s="26"/>
+      <c r="B390" s="29"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="26" t="s">
+      <c r="A391" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="B391" s="26"/>
+      <c r="B391" s="29"/>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="26" t="s">
+      <c r="A392" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="B392" s="26"/>
+      <c r="B392" s="29"/>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="26" t="s">
+      <c r="A393" s="29" t="s">
         <v>417</v>
       </c>
-      <c r="B393" s="27" t="s">
+      <c r="B393" s="30" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="26" t="s">
+      <c r="A394" s="29" t="s">
         <v>418</v>
       </c>
-      <c r="B394" s="27" t="s">
+      <c r="B394" s="30" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="26" t="s">
+      <c r="A395" s="29" t="s">
         <v>419</v>
       </c>
-      <c r="B395" s="26"/>
+      <c r="B395" s="29"/>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="26" t="s">
+      <c r="A396" s="29" t="s">
         <v>420</v>
       </c>
-      <c r="B396" s="26"/>
+      <c r="B396" s="29"/>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="26" t="s">
+      <c r="A397" s="29" t="s">
         <v>421</v>
       </c>
-      <c r="B397" s="26"/>
+      <c r="B397" s="29"/>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="24" t="s">
+      <c r="A398" s="27" t="s">
         <v>422</v>
       </c>
-      <c r="B398" s="26"/>
+      <c r="B398" s="29"/>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="24" t="s">
+      <c r="A399" s="27" t="s">
         <v>423</v>
       </c>
-      <c r="B399" s="26"/>
+      <c r="B399" s="29"/>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="24" t="s">
+      <c r="A400" s="27" t="s">
         <v>424</v>
       </c>
-      <c r="B400" s="25" t="s">
+      <c r="B400" s="28" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="24" t="s">
+      <c r="A401" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="B401" s="25" t="s">
+      <c r="B401" s="28" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="24" t="s">
+      <c r="A402" s="27" t="s">
         <v>426</v>
       </c>
-      <c r="B402" s="26"/>
+      <c r="B402" s="29"/>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="24" t="s">
+      <c r="A403" s="27" t="s">
         <v>427</v>
       </c>
-      <c r="B403" s="26"/>
+      <c r="B403" s="29"/>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="24" t="s">
+      <c r="A404" s="27" t="s">
         <v>428</v>
       </c>
-      <c r="B404" s="26"/>
+      <c r="B404" s="29"/>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="24" t="s">
+      <c r="A405" s="27" t="s">
         <v>429</v>
       </c>
-      <c r="B405" s="26"/>
+      <c r="B405" s="29"/>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="24" t="s">
+      <c r="A406" s="27" t="s">
         <v>430</v>
       </c>
-      <c r="B406" s="26"/>
+      <c r="B406" s="29"/>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="24" t="s">
+      <c r="A407" s="27" t="s">
         <v>431</v>
       </c>
-      <c r="B407" s="25" t="s">
+      <c r="B407" s="28" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="24" t="s">
+      <c r="A408" s="27" t="s">
         <v>432</v>
       </c>
-      <c r="B408" s="25" t="s">
+      <c r="B408" s="28" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="24" t="s">
+      <c r="A409" s="27" t="s">
         <v>433</v>
       </c>
-      <c r="B409" s="26"/>
+      <c r="B409" s="29"/>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="26" t="s">
+      <c r="A410" s="29" t="s">
         <v>434</v>
       </c>
-      <c r="B410" s="26"/>
+      <c r="B410" s="29"/>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="26" t="s">
+      <c r="A411" s="29" t="s">
         <v>435</v>
       </c>
-      <c r="B411" s="26"/>
+      <c r="B411" s="29"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="26" t="s">
+      <c r="A412" s="29" t="s">
         <v>436</v>
       </c>
-      <c r="B412" s="26"/>
+      <c r="B412" s="29"/>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="26" t="s">
+      <c r="A413" s="29" t="s">
         <v>437</v>
       </c>
-      <c r="B413" s="26"/>
+      <c r="B413" s="29"/>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="26" t="s">
+      <c r="A414" s="29" t="s">
         <v>438</v>
       </c>
-      <c r="B414" s="27" t="s">
+      <c r="B414" s="30" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="26" t="s">
+      <c r="A415" s="29" t="s">
         <v>439</v>
       </c>
-      <c r="B415" s="27" t="s">
+      <c r="B415" s="30" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="26" t="s">
+      <c r="A416" s="29" t="s">
         <v>440</v>
       </c>
-      <c r="B416" s="26"/>
+      <c r="B416" s="29"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="26" t="s">
+      <c r="A417" s="29" t="s">
         <v>441</v>
       </c>
-      <c r="B417" s="26"/>
+      <c r="B417" s="29"/>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="26" t="s">
+      <c r="A418" s="29" t="s">
         <v>442</v>
       </c>
-      <c r="B418" s="26"/>
+      <c r="B418" s="29"/>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="26" t="s">
+      <c r="A419" s="29" t="s">
         <v>443</v>
       </c>
-      <c r="B419" s="26"/>
+      <c r="B419" s="29"/>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="26" t="s">
+      <c r="A420" s="29" t="s">
         <v>444</v>
       </c>
-      <c r="B420" s="26"/>
+      <c r="B420" s="29"/>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="26" t="s">
+      <c r="A421" s="29" t="s">
         <v>445</v>
       </c>
-      <c r="B421" s="27" t="s">
+      <c r="B421" s="30" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="26" t="s">
+      <c r="A422" s="29" t="s">
         <v>446</v>
       </c>
-      <c r="B422" s="27" t="s">
+      <c r="B422" s="30" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="26" t="s">
+      <c r="A423" s="29" t="s">
         <v>447</v>
       </c>
-      <c r="B423" s="26"/>
+      <c r="B423" s="29"/>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="26" t="s">
+      <c r="A424" s="29" t="s">
         <v>448</v>
       </c>
-      <c r="B424" s="26"/>
+      <c r="B424" s="29"/>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="26" t="s">
+      <c r="A425" s="29" t="s">
         <v>449</v>
       </c>
-      <c r="B425" s="26"/>
+      <c r="B425" s="29"/>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="24" t="s">
+      <c r="A426" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="B426" s="26"/>
+      <c r="B426" s="29"/>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="24" t="s">
+      <c r="A427" s="27" t="s">
         <v>451</v>
       </c>
-      <c r="B427" s="26"/>
+      <c r="B427" s="29"/>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="24" t="s">
+      <c r="A428" s="27" t="s">
         <v>452</v>
       </c>
-      <c r="B428" s="25" t="s">
+      <c r="B428" s="28" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="24" t="s">
+      <c r="A429" s="27" t="s">
         <v>453</v>
       </c>
-      <c r="B429" s="25" t="s">
+      <c r="B429" s="28" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="24" t="s">
+      <c r="A430" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="B430" s="26"/>
+      <c r="B430" s="29"/>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="24" t="s">
+      <c r="A431" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="B431" s="26"/>
+      <c r="B431" s="29"/>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="24" t="s">
+      <c r="A432" s="27" t="s">
         <v>456</v>
       </c>
-      <c r="B432" s="26"/>
+      <c r="B432" s="29"/>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="24" t="s">
+      <c r="A433" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="B433" s="26"/>
+      <c r="B433" s="29"/>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="24" t="s">
+      <c r="A434" s="27" t="s">
         <v>458</v>
       </c>
-      <c r="B434" s="26"/>
+      <c r="B434" s="29"/>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="24" t="s">
+      <c r="A435" s="27" t="s">
         <v>459</v>
       </c>
-      <c r="B435" s="25" t="s">
+      <c r="B435" s="28" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="24" t="s">
+      <c r="A436" s="27" t="s">
         <v>460</v>
       </c>
-      <c r="B436" s="25" t="s">
+      <c r="B436" s="28" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="24" t="s">
+      <c r="A437" s="27" t="s">
         <v>461</v>
       </c>
-      <c r="B437" s="26"/>
+      <c r="B437" s="29"/>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="26" t="s">
+      <c r="A438" s="29" t="s">
         <v>462</v>
       </c>
-      <c r="B438" s="26"/>
+      <c r="B438" s="29"/>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="26" t="s">
+      <c r="A439" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="B439" s="26"/>
+      <c r="B439" s="29"/>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="26" t="s">
+      <c r="A440" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="B440" s="26"/>
+      <c r="B440" s="29"/>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="26" t="s">
+      <c r="A441" s="29" t="s">
         <v>465</v>
       </c>
-      <c r="B441" s="26"/>
+      <c r="B441" s="29"/>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="26" t="s">
+      <c r="A442" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="B442" s="27" t="s">
+      <c r="B442" s="30" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="26" t="s">
+      <c r="A443" s="29" t="s">
         <v>467</v>
       </c>
-      <c r="B443" s="27" t="s">
+      <c r="B443" s="30" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="26" t="s">
+      <c r="A444" s="29" t="s">
         <v>468</v>
       </c>
-      <c r="B444" s="26"/>
+      <c r="B444" s="29"/>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="26" t="s">
+      <c r="A445" s="29" t="s">
         <v>469</v>
       </c>
-      <c r="B445" s="26"/>
+      <c r="B445" s="29"/>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="26" t="s">
+      <c r="A446" s="29" t="s">
         <v>470</v>
       </c>
-      <c r="B446" s="26"/>
+      <c r="B446" s="29"/>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="26" t="s">
+      <c r="A447" s="29" t="s">
         <v>471</v>
       </c>
-      <c r="B447" s="26"/>
+      <c r="B447" s="29"/>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="26" t="s">
+      <c r="A448" s="29" t="s">
         <v>472</v>
       </c>
-      <c r="B448" s="26"/>
+      <c r="B448" s="29"/>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="26" t="s">
+      <c r="A449" s="29" t="s">
         <v>473</v>
       </c>
-      <c r="B449" s="27" t="s">
+      <c r="B449" s="30" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="26" t="s">
+      <c r="A450" s="29" t="s">
         <v>474</v>
       </c>
-      <c r="B450" s="27" t="s">
+      <c r="B450" s="30" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="26" t="s">
+      <c r="A451" s="29" t="s">
         <v>475</v>
       </c>
-      <c r="B451" s="26"/>
+      <c r="B451" s="29"/>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="26" t="s">
+      <c r="A452" s="29" t="s">
         <v>476</v>
       </c>
-      <c r="B452" s="26"/>
+      <c r="B452" s="29"/>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="26" t="s">
+      <c r="A453" s="29" t="s">
         <v>477</v>
       </c>
-      <c r="B453" s="26"/>
+      <c r="B453" s="29"/>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="26" t="s">
+      <c r="A454" s="29" t="s">
         <v>478</v>
       </c>
-      <c r="B454" s="26"/>
+      <c r="B454" s="29"/>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="26" t="s">
+      <c r="A455" s="29" t="s">
         <v>479</v>
       </c>
-      <c r="B455" s="26"/>
+      <c r="B455" s="29"/>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="26" t="s">
+      <c r="A456" s="29" t="s">
         <v>480</v>
       </c>
-      <c r="B456" s="27" t="s">
+      <c r="B456" s="30" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="24" t="s">
+      <c r="A457" s="27" t="s">
         <v>481</v>
       </c>
-      <c r="B457" s="25" t="s">
+      <c r="B457" s="28" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="24" t="s">
+      <c r="A458" s="27" t="s">
         <v>482</v>
       </c>
-      <c r="B458" s="26"/>
+      <c r="B458" s="29"/>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="24" t="s">
+      <c r="A459" s="27" t="s">
         <v>483</v>
       </c>
-      <c r="B459" s="26"/>
+      <c r="B459" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -14227,7 +14240,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>